<commit_message>
[IMP] Adjust Budget Report
</commit_message>
<xml_diff>
--- a/pabi_budget_report/xlsx_template/xlsx_report_budget_plan_construction_analysis.xlsx
+++ b/pabi_budget_report/xlsx_template/xlsx_report_budget_plan_construction_analysis.xlsx
@@ -286,8 +286,8 @@
   </sheetPr>
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -296,7 +296,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.19"/>

</xml_diff>